<commit_message>
added moment of inertia
</commit_message>
<xml_diff>
--- a/labs/lab4/Report/lab4ee155.xlsx
+++ b/labs/lab4/Report/lab4ee155.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Data</t>
   </si>
@@ -109,6 +109,45 @@
   </si>
   <si>
     <t>current max power</t>
+  </si>
+  <si>
+    <t>40ms window</t>
+  </si>
+  <si>
+    <t>t=0</t>
+  </si>
+  <si>
+    <t>t=40ms</t>
+  </si>
+  <si>
+    <t>rms current</t>
+  </si>
+  <si>
+    <t>LCR max</t>
+  </si>
+  <si>
+    <t>2.7mH</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>Measurement of Moment of Inertia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torque </t>
+  </si>
+  <si>
+    <t>2*ms</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>rad/s^2</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1746,7 +1785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:21">
       <c r="A17">
         <v>20</v>
       </c>
@@ -1781,7 +1820,7 @@
         <v>628.31853071795865</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:21">
       <c r="A18">
         <v>22</v>
       </c>
@@ -1816,7 +1855,7 @@
         <v>766.24211063165694</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:21">
       <c r="A19">
         <v>23</v>
       </c>
@@ -1851,7 +1890,7 @@
         <v>835.52996106111516</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:21">
       <c r="A20">
         <v>24</v>
       </c>
@@ -1884,6 +1923,125 @@
       <c r="I20">
         <f t="shared" si="4"/>
         <v>882.46984651398679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="Q21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="Q24" t="s">
+        <v>30</v>
+      </c>
+      <c r="R24" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" t="s">
+        <v>39</v>
+      </c>
+      <c r="T24" t="s">
+        <v>6</v>
+      </c>
+      <c r="U24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="Q25" t="s">
+        <v>31</v>
+      </c>
+      <c r="R25">
+        <v>9.4</v>
+      </c>
+      <c r="S25">
+        <f>R25*2</f>
+        <v>18.8</v>
+      </c>
+      <c r="T25">
+        <f>1/S25*1000</f>
+        <v>53.191489361702125</v>
+      </c>
+      <c r="U25">
+        <f>2*PI()*T25</f>
+        <v>334.21198442444609</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="Q26" t="s">
+        <v>32</v>
+      </c>
+      <c r="R26">
+        <v>4</v>
+      </c>
+      <c r="S26">
+        <f>R26*2</f>
+        <v>8</v>
+      </c>
+      <c r="T26">
+        <f>1/S26*1000</f>
+        <v>125</v>
+      </c>
+      <c r="U26">
+        <f>2*PI()*T26</f>
+        <v>785.39816339744823</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="Q28" t="s">
+        <v>33</v>
+      </c>
+      <c r="R28">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="Q31" t="s">
+        <v>34</v>
+      </c>
+      <c r="R31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="Q32" t="s">
+        <v>36</v>
+      </c>
+      <c r="R32">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="17:19">
+      <c r="Q35" t="s">
+        <v>38</v>
+      </c>
+      <c r="R35">
+        <f>R28/R3</f>
+        <v>103.3210332103321</v>
+      </c>
+      <c r="S35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="17:19">
+      <c r="Q36" t="s">
+        <v>40</v>
+      </c>
+      <c r="R36">
+        <f>(U26-U25)/0.04</f>
+        <v>11279.654474325052</v>
+      </c>
+      <c r="S36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="17:19">
+      <c r="Q38" t="s">
+        <v>41</v>
+      </c>
+      <c r="R38">
+        <f>R35/R36</f>
+        <v>9.1599466495638892E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>